<commit_message>
added penalty for bad plate
</commit_message>
<xml_diff>
--- a/files/input_fake.xlsx
+++ b/files/input_fake.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="47">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">glycerol</t>
   </si>
   <si>
+    <t xml:space="preserve">testable?</t>
+  </si>
+  <si>
     <t xml:space="preserve">density</t>
   </si>
   <si>
@@ -67,6 +70,9 @@
     <t xml:space="preserve">Olive stone</t>
   </si>
   <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">RecellCal100</t>
   </si>
   <si>
@@ -149,6 +155,9 @@
   </si>
   <si>
     <t xml:space="preserve">Sto2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
   </si>
   <si>
     <t xml:space="preserve">Sto2.15</t>
@@ -263,13 +272,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ27"/>
+  <dimension ref="A1:AMJ26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.36"/>
@@ -313,16 +322,19 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0.0925</v>
@@ -336,31 +348,34 @@
       <c r="G2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="0" t="n">
         <v>1.43203368521146</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="J2" s="0" t="n">
         <v>1.8</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="K2" s="0" t="n">
         <v>11.7</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="L2" s="0" t="n">
         <v>32.7</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="M2" s="0" t="n">
         <v>4420</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0.0925</v>
@@ -374,31 +389,34 @@
       <c r="G3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="0" t="n">
         <v>2.00341700000452</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="J3" s="0" t="n">
         <v>2.8</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="K3" s="0" t="n">
         <v>12.7</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="L3" s="0" t="n">
         <v>42.45</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="M3" s="0" t="n">
         <v>4770</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0.15</v>
@@ -412,31 +430,34 @@
       <c r="G4" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="0" t="n">
         <v>1.63069084890505</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="J4" s="0" t="n">
         <v>3.8</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="K4" s="0" t="n">
         <v>13.7</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="L4" s="0" t="n">
         <v>37.36</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="M4" s="0" t="n">
         <v>4318</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0.15</v>
@@ -450,31 +471,34 @@
       <c r="G5" s="0" t="n">
         <v>0.0384</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="0" t="n">
         <v>1.63069084890505</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="J5" s="0" t="n">
         <v>4.8</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="K5" s="0" t="n">
         <v>14.7</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="L5" s="0" t="n">
         <v>38.65</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="M5" s="0" t="n">
         <v>3930</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>0.1075</v>
@@ -488,31 +512,34 @@
       <c r="G6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="0" t="n">
         <v>1.78648495833704</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="J6" s="0" t="n">
         <v>5.8</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="K6" s="0" t="n">
         <v>15.7</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="L6" s="0" t="n">
         <v>39.65</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="M6" s="0" t="n">
         <v>3931</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>0.0995</v>
@@ -526,31 +553,34 @@
       <c r="G7" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="H7" s="2" t="n">
+      <c r="H7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="2" t="n">
         <v>1.98488465214295</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="J7" s="0" t="n">
         <v>6.8</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="K7" s="0" t="n">
         <v>16.7</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="L7" s="0" t="n">
         <v>40.65</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="M7" s="0" t="n">
         <v>3932</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>0.1169</v>
@@ -564,31 +594,34 @@
       <c r="G8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="H8" s="2" t="n">
+      <c r="H8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="2" t="n">
         <v>1.64207328751883</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="J8" s="0" t="n">
         <v>7.8</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="K8" s="0" t="n">
         <v>17.7</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="L8" s="0" t="n">
         <v>41.65</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="M8" s="0" t="n">
         <v>3933</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>0.1515</v>
@@ -602,31 +635,34 @@
       <c r="G9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H9" s="2" t="n">
+      <c r="H9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="2" t="n">
         <v>2.11906872193506</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="J9" s="0" t="n">
         <v>8.8</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="K9" s="0" t="n">
         <v>2.7</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="L9" s="0" t="n">
         <v>35.3</v>
       </c>
-      <c r="L9" s="0" t="n">
+      <c r="M9" s="0" t="n">
         <v>3934</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>0.1111</v>
@@ -640,31 +676,34 @@
       <c r="G10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="0" t="n">
         <v>1.97504272193506</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="J10" s="0" t="n">
         <v>6.6</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="K10" s="0" t="n">
         <v>3.7</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="L10" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="L10" s="0" t="n">
+      <c r="M10" s="0" t="n">
         <v>3935</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>0.0925</v>
@@ -678,31 +717,34 @@
       <c r="G11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="0" t="n">
         <v>2.15604200000452</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="J11" s="0" t="n">
         <v>7.6</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="K11" s="0" t="n">
         <v>4.7</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="L11" s="0" t="n">
         <v>27.8</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="M11" s="0" t="n">
         <v>3936</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>0.0808</v>
@@ -716,31 +758,34 @@
       <c r="G12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="0" t="n">
         <v>2.18976872193506</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="J12" s="0" t="n">
         <v>9.8</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="K12" s="0" t="n">
         <v>5.7</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="L12" s="0" t="n">
         <v>28.8</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="M12" s="0" t="n">
         <v>3937</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>0.1111</v>
@@ -754,34 +799,36 @@
       <c r="G13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="0" t="n">
         <v>2.15946872193506</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="J13" s="0" t="n">
         <v>9.4</v>
       </c>
-      <c r="J13" s="0" t="n">
+      <c r="K13" s="0" t="n">
         <v>6.7</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="L13" s="0" t="n">
         <v>33.6</v>
       </c>
-      <c r="L13" s="0" t="n">
+      <c r="M13" s="0" t="n">
         <v>3938</v>
       </c>
-      <c r="AMH13" s="0"/>
       <c r="AMI13" s="0"/>
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>0.0889</v>
@@ -795,34 +842,36 @@
       <c r="G14" s="0" t="n">
         <v>0.0384</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="0" t="n">
         <v>1.96869549213507</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="J14" s="0" t="n">
         <v>10.4</v>
       </c>
-      <c r="J14" s="0" t="n">
+      <c r="K14" s="0" t="n">
         <v>7.7</v>
       </c>
-      <c r="K14" s="0" t="n">
+      <c r="L14" s="0" t="n">
         <v>39.76</v>
       </c>
-      <c r="L14" s="2" t="n">
+      <c r="M14" s="2" t="n">
         <v>7516</v>
       </c>
-      <c r="AMH14" s="0"/>
       <c r="AMI14" s="0"/>
       <c r="AMJ14" s="0"/>
     </row>
     <row r="15" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>0.15</v>
@@ -836,34 +885,36 @@
       <c r="G15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="0" t="n">
         <v>1.02560584890505</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="J15" s="0" t="n">
         <v>11.4</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="K15" s="0" t="n">
         <v>8.7</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="L15" s="0" t="n">
         <v>42.4</v>
       </c>
-      <c r="L15" s="2" t="n">
+      <c r="M15" s="2" t="n">
         <v>4770</v>
       </c>
-      <c r="AMH15" s="0"/>
       <c r="AMI15" s="0"/>
       <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>0.1026</v>
@@ -877,31 +928,34 @@
       <c r="G16" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="0" t="n">
         <v>2.09828669765034</v>
       </c>
-      <c r="I16" s="0" t="n">
+      <c r="J16" s="0" t="n">
         <v>12.4</v>
       </c>
-      <c r="J16" s="0" t="n">
+      <c r="K16" s="0" t="n">
         <v>9.7</v>
       </c>
-      <c r="K16" s="0" t="n">
+      <c r="L16" s="0" t="n">
         <v>47.9</v>
       </c>
-      <c r="L16" s="2" t="n">
+      <c r="M16" s="2" t="n">
         <v>2024</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>0.1151</v>
@@ -915,31 +969,34 @@
       <c r="G17" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="0" t="n">
         <v>2.02664780678631</v>
       </c>
-      <c r="I17" s="0" t="n">
+      <c r="J17" s="0" t="n">
         <v>13.4</v>
       </c>
-      <c r="J17" s="0" t="n">
+      <c r="K17" s="0" t="n">
         <v>10.7</v>
       </c>
-      <c r="K17" s="0" t="n">
+      <c r="L17" s="0" t="n">
         <v>48.6</v>
       </c>
-      <c r="L17" s="2" t="n">
+      <c r="M17" s="2" t="n">
         <v>2025</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>0.131</v>
@@ -953,31 +1010,34 @@
       <c r="G18" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="0" t="n">
         <v>1.9350599444681</v>
       </c>
-      <c r="I18" s="0" t="n">
+      <c r="J18" s="0" t="n">
         <v>14.4</v>
       </c>
-      <c r="J18" s="0" t="n">
+      <c r="K18" s="0" t="n">
         <v>11.7</v>
       </c>
-      <c r="K18" s="0" t="n">
+      <c r="L18" s="0" t="n">
         <v>53.9</v>
       </c>
-      <c r="L18" s="2" t="n">
+      <c r="M18" s="2" t="n">
         <v>2026</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>0.0925</v>
@@ -991,31 +1051,34 @@
       <c r="G19" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="0" t="n">
         <v>1.46762868521146</v>
       </c>
-      <c r="I19" s="0" t="n">
+      <c r="J19" s="0" t="n">
         <v>15.4</v>
       </c>
-      <c r="J19" s="0" t="n">
+      <c r="K19" s="0" t="n">
         <v>12.7</v>
       </c>
-      <c r="K19" s="0" t="n">
+      <c r="L19" s="0" t="n">
         <v>54.9</v>
       </c>
-      <c r="L19" s="2" t="n">
+      <c r="M19" s="2" t="n">
         <v>2027</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>0.0925</v>
@@ -1029,31 +1092,34 @@
       <c r="G20" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="0" t="n">
         <v>1.31832943075185</v>
       </c>
-      <c r="I20" s="0" t="n">
+      <c r="J20" s="0" t="n">
         <v>16.4</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="K20" s="0" t="n">
         <v>13.7</v>
       </c>
-      <c r="K20" s="0" t="n">
+      <c r="L20" s="0" t="n">
         <v>55.9</v>
       </c>
-      <c r="L20" s="2" t="n">
+      <c r="M20" s="2" t="n">
         <v>2028</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>0.0925</v>
@@ -1067,31 +1133,34 @@
       <c r="G21" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="0" t="n">
         <v>1.71873900000452</v>
       </c>
-      <c r="I21" s="0" t="n">
+      <c r="J21" s="0" t="n">
         <v>17.4</v>
       </c>
-      <c r="J21" s="0" t="n">
+      <c r="K21" s="0" t="n">
         <v>14.7</v>
       </c>
-      <c r="K21" s="0" t="n">
+      <c r="L21" s="0" t="n">
         <v>56.9</v>
       </c>
-      <c r="L21" s="2" t="n">
+      <c r="M21" s="2" t="n">
         <v>2029</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>0.0925</v>
@@ -1105,31 +1174,34 @@
       <c r="G22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="0" t="n">
         <v>1.49962500000452</v>
       </c>
-      <c r="I22" s="0" t="n">
+      <c r="J22" s="0" t="n">
         <v>18.4</v>
       </c>
-      <c r="J22" s="0" t="n">
+      <c r="K22" s="0" t="n">
         <v>15.7</v>
       </c>
-      <c r="K22" s="0" t="n">
+      <c r="L22" s="0" t="n">
         <v>57.9</v>
       </c>
-      <c r="L22" s="2" t="n">
+      <c r="M22" s="2" t="n">
         <v>2030</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>0.1492</v>
@@ -1143,31 +1215,34 @@
       <c r="G23" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="H23" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="0" t="n">
         <v>1.26387545226369</v>
       </c>
-      <c r="I23" s="0" t="n">
+      <c r="J23" s="0" t="n">
         <v>19.4</v>
       </c>
-      <c r="J23" s="0" t="n">
+      <c r="K23" s="0" t="n">
         <v>16.7</v>
       </c>
-      <c r="K23" s="0" t="n">
+      <c r="L23" s="0" t="n">
         <v>32.74</v>
       </c>
-      <c r="L23" s="0" t="n">
+      <c r="M23" s="0" t="n">
         <v>3933</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>0.202</v>
@@ -1181,31 +1256,34 @@
       <c r="G24" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="0" t="n">
         <v>2.06856872193506</v>
       </c>
-      <c r="I24" s="0" t="n">
+      <c r="J24" s="0" t="n">
         <v>8.5</v>
       </c>
-      <c r="J24" s="0" t="n">
+      <c r="K24" s="0" t="n">
         <v>17.7</v>
       </c>
-      <c r="K24" s="0" t="n">
+      <c r="L24" s="0" t="n">
         <v>30.4</v>
       </c>
-      <c r="L24" s="0" t="n">
+      <c r="M24" s="0" t="n">
         <v>3934</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>0.0808</v>
@@ -1219,95 +1297,48 @@
       <c r="G25" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H25" s="0" t="n">
-        <v>2.05564072193506</v>
-      </c>
-      <c r="I25" s="0" t="n">
-        <v>10.5</v>
-      </c>
-      <c r="J25" s="0" t="n">
-        <v>18.7</v>
-      </c>
-      <c r="K25" s="0" t="n">
-        <v>44.3</v>
-      </c>
-      <c r="L25" s="0" t="n">
-        <v>3935</v>
+      <c r="H25" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>0.1111</v>
+        <v>0.0918</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>0.7272</v>
+        <v>0.7245</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H26" s="0" t="n">
-        <v>1.97504272193506</v>
+      <c r="H26" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="I26" s="0" t="n">
-        <v>6.6</v>
+        <v>2.02203151207151</v>
       </c>
       <c r="J26" s="0" t="n">
-        <v>19.7</v>
+        <v>9.7</v>
       </c>
       <c r="K26" s="0" t="n">
-        <v>42</v>
+        <v>2.1</v>
       </c>
       <c r="L26" s="0" t="n">
-        <v>3936</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="0" t="n">
-        <v>0.0918</v>
-      </c>
-      <c r="E27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" s="0" t="n">
-        <v>0.7245</v>
-      </c>
-      <c r="G27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="0" t="n">
-        <v>2.02203151207151</v>
-      </c>
-      <c r="I27" s="0" t="n">
-        <v>9.7</v>
-      </c>
-      <c r="J27" s="0" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="K27" s="0" t="n">
         <v>40.4</v>
       </c>
-      <c r="L27" s="0" t="n">
+      <c r="M26" s="0" t="n">
         <v>7080</v>
       </c>
     </row>

</xml_diff>